<commit_message>
portfolio_hedge.py added.  dash_risk_grid.py add hedge ratio display
</commit_message>
<xml_diff>
--- a/dashrisk/min_variance.xlsx
+++ b/dashrisk/min_variance.xlsx
@@ -12,8 +12,8 @@
     <workbookView xWindow="1840" yWindow="2680" windowWidth="23720" windowHeight="14480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="df_hist_portfolio_hedge" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="spy_vs_ets" sheetId="1" r:id="rId1"/>
+    <sheet name="min_variance_hedge" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -386,7 +386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K103"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A98" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -4004,7 +4004,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>

</xml_diff>